<commit_message>
Updated README to include new directory structure
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pamelagreen/Desktop/Data/SustSolutionOpp/scripts/OppMap_main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FB8C33-0FC3-B648-9341-D8DDAE2D6852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BAAED3-CDBF-F14F-BE26-1B8B83D78534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45340" yWindow="-680" windowWidth="31580" windowHeight="20260" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
+    <workbookView xWindow="41380" yWindow="-680" windowWidth="31580" windowHeight="20260" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="225">
   <si>
     <r>
       <rPr>
@@ -1137,6 +1137,12 @@
     </r>
   </si>
   <si>
+    <t>Authors: Pamela Green</t>
+  </si>
+  <si>
+    <t>Contact: pg@pamelaagreen.com</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1156,14 +1162,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: lists model output files contained in the zip files 'Model_Output-GII.zip, Model_Output-IWRM.zip, Model_Output-AdaptiveCapacity.zip'</t>
-    </r>
-  </si>
-  <si>
-    <t>Authors: Pamela Green</t>
-  </si>
-  <si>
-    <t>Contact: pg@pamelaagreen.com</t>
+      <t>: lists model output files contained in the zip files 'Model_Output-WSN.zip, Model_Output-GII.zip, Model_Output-IWRM.zip, Model_Output-AdaptiveCapacity.zip'</t>
+    </r>
+  </si>
+  <si>
+    <t>Model_Output/rasters/WSN</t>
+  </si>
+  <si>
+    <t>Model_Output/rasters/GII</t>
+  </si>
+  <si>
+    <t>Enabling Environment for GII, IWRM and Adaptive Capacity</t>
+  </si>
+  <si>
+    <t>Enabling_Environment_IWRM.tif</t>
+  </si>
+  <si>
+    <t>Model_Output/rasters/IWRM</t>
+  </si>
+  <si>
+    <t>IWRM rescaled scores mapped to GADM country boundaries</t>
+  </si>
+  <si>
+    <t>Adaptive Capacity rescaled scores mapped to GADM country boundaries</t>
+  </si>
+  <si>
+    <t>Enabling_Environment_AdaptiveCap.tif</t>
+  </si>
+  <si>
+    <t>Model_Output/rasters/AdaptiveCap</t>
   </si>
 </sst>
 </file>
@@ -1645,12 +1672,12 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="136.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="149.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.3">
@@ -1665,12 +1692,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -1710,7 +1737,7 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2143,10 +2170,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998D523C-B220-F44C-B515-B79245E7605B}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView topLeftCell="A74" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2180,7 +2207,7 @@
         <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -2197,7 +2224,7 @@
         <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>217</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -2275,7 +2302,7 @@
         <v>204</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>216</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -2292,7 +2319,7 @@
         <v>205</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>216</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -2309,7 +2336,7 @@
         <v>206</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>216</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -3263,6 +3290,62 @@
       </c>
       <c r="D109" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="13" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>141</v>
+      </c>
+      <c r="B112" t="s">
+        <v>217</v>
+      </c>
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" t="s">
+        <v>46</v>
+      </c>
+      <c r="E112" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" t="s">
+        <v>220</v>
+      </c>
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" t="s">
+        <v>46</v>
+      </c>
+      <c r="E113" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>223</v>
+      </c>
+      <c r="B114" t="s">
+        <v>224</v>
+      </c>
+      <c r="C114" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" t="s">
+        <v>46</v>
+      </c>
+      <c r="E114" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>